<commit_message>
Ticket 60 - XSSF templates with comments have indexed color 81 defined, which doesn't exist.  Account for that possibility in ExcelColor.
</commit_message>
<xml_diff>
--- a/jett-core/templates/CommentTagTemplate.xlsx
+++ b/jett-core/templates/CommentTagTemplate.xlsx
@@ -11,6 +11,40 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Gettman, Randy</author>
+  </authors>
+  <commentList>
+    <comment ref="H12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Color #81</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ticket #60</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -94,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +143,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -637,8 +684,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -650,7 +697,7 @@
     <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -658,7 +705,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -672,7 +719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -686,11 +733,13 @@
         <v>7</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>